<commit_message>
Coupling changes between soil and root-cynaps (1e10476882bf61060088a713c5a04d4662c77335)
</commit_message>
<xml_diff>
--- a/simulations/single_plant/inputs/Scenarios_24-11-06.xlsx
+++ b/simulations/single_plant/inputs/Scenarios_24-11-06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sshfs\torisuten@192.168.12.9\package\Wheat-BRIDGES\simulations\single_plant\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A7C0F5-C782-4C8D-BFA2-2764FDC9781F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E21F56-18FC-4053-BAE8-39AB0EB9BFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-48120" yWindow="4200" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2885,7 +2885,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
+      <selection pane="bottomRight" activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5472,7 +5472,7 @@
         <v>3</v>
       </c>
       <c r="R19" s="44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S19" s="44">
         <v>3</v>

</xml_diff>